<commit_message>
Librarian and Customer done. Started Check in
</commit_message>
<xml_diff>
--- a/Homework 11/Product Backlog.xlsx
+++ b/Homework 11/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/aaa2575_HW10/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/Repositories/1325-repository/Homework 11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{57D7FE39-D326-C743-86A0-D11D9AD09887}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{521BD598-1268-554C-9059-7027A6704E95}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1780" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44800" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="202">
   <si>
     <t>Product Name:</t>
   </si>
@@ -600,6 +600,42 @@
   </si>
   <si>
     <t>Prints out all media in a dialog box</t>
+  </si>
+  <si>
+    <t>Create Dialog box to allow librarians to be created via GUI</t>
+  </si>
+  <si>
+    <t>Allow Librarians to be created via GUI</t>
+  </si>
+  <si>
+    <t>Create Dialog box to allow customers to be created via GUI</t>
+  </si>
+  <si>
+    <t>Allow Customers to be created via GUI</t>
+  </si>
+  <si>
+    <t>Create Dialog box to allow Check in via GUI</t>
+  </si>
+  <si>
+    <t>Allow Customers to check in media via GUI</t>
+  </si>
+  <si>
+    <t>Create Dialog box to allow Check out via GUI</t>
+  </si>
+  <si>
+    <t>Allows Customers to check out media via GUI</t>
+  </si>
+  <si>
+    <t>Create Dialog box to allow customers to pay balance via GUI</t>
+  </si>
+  <si>
+    <t>Allows Customers to pay a balance via GUI</t>
+  </si>
+  <si>
+    <t>Allow the Library Manament system to utilize a menu bar for various functions</t>
+  </si>
+  <si>
+    <t>Implement a menu bar</t>
   </si>
 </sst>
 </file>
@@ -2561,28 +2597,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7159,8 +7195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9967,8 +10003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:XFD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10225,21 +10261,24 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10272,7 +10311,7 @@
       </c>
       <c r="B5">
         <f>COUNT(A15:A1000)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -10281,7 +10320,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B12" si="0">B5</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -10290,7 +10329,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -10299,7 +10338,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -10308,7 +10347,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -10317,7 +10356,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -10326,7 +10365,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -10335,7 +10374,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -10362,6 +10401,176 @@
       </c>
       <c r="H17" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" t="s">
+        <v>193</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <f t="shared" ref="A20:A24" si="1">A19+1</f>
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" t="s">
+        <v>182</v>
+      </c>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" t="s">
+        <v>195</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C23" t="s">
+        <v>182</v>
+      </c>
+      <c r="D23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" t="s">
+        <v>200</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>139</v>
+      </c>
+      <c r="G24" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Media check in complete
</commit_message>
<xml_diff>
--- a/Homework 11/Product Backlog.xlsx
+++ b/Homework 11/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/Repositories/1325-repository/Homework 11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{521BD598-1268-554C-9059-7027A6704E95}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13B689FD-FD57-2141-B154-320A7835A24D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44800" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3720" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="203">
   <si>
     <t>Product Name:</t>
   </si>
@@ -636,6 +636,9 @@
   </si>
   <si>
     <t>Implement a menu bar</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -7195,8 +7198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7839,7 +7842,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="D34" s="4">
         <v>4</v>
@@ -7866,7 +7869,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="D35" s="4">
         <v>4</v>
@@ -7893,7 +7896,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="D36" s="4">
         <v>4</v>
@@ -7920,7 +7923,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
       <c r="D37" s="4">
         <v>4</v>
@@ -10270,8 +10273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -10423,7 +10426,7 @@
         <v>191</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -10447,7 +10450,7 @@
         <v>193</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -10471,7 +10474,7 @@
         <v>195</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -10495,7 +10498,7 @@
         <v>197</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -10567,7 +10570,7 @@
         <v>139</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
       <c r="H24" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
Finished check in function using GUI
</commit_message>
<xml_diff>
--- a/Homework 11/Product Backlog.xlsx
+++ b/Homework 11/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/Repositories/1325-repository/Homework 11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13B689FD-FD57-2141-B154-320A7835A24D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B5AC9E48-484B-5D4B-9C67-88EFC5B89B21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="199">
   <si>
     <t>Product Name:</t>
   </si>
@@ -575,70 +575,58 @@
     <t>Need to fix check in and check out for transaction</t>
   </si>
   <si>
-    <t>Create Dialog class to handle interations with GUI</t>
-  </si>
-  <si>
     <t>CD</t>
   </si>
   <si>
     <t xml:space="preserve">Allow GUI to interact with current classes </t>
   </si>
   <si>
-    <t>Create Dialog box which opens the main gui window</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allow customers to see main window </t>
   </si>
   <si>
-    <t>Allow users to select the create bundles and media option and then call gui</t>
-  </si>
-  <si>
     <t xml:space="preserve">Allow GUI selection of different menu items </t>
   </si>
   <si>
-    <t>Print out all available media in a GUI</t>
-  </si>
-  <si>
     <t>Prints out all media in a dialog box</t>
   </si>
   <si>
-    <t>Create Dialog box to allow librarians to be created via GUI</t>
-  </si>
-  <si>
     <t>Allow Librarians to be created via GUI</t>
   </si>
   <si>
-    <t>Create Dialog box to allow customers to be created via GUI</t>
-  </si>
-  <si>
     <t>Allow Customers to be created via GUI</t>
   </si>
   <si>
-    <t>Create Dialog box to allow Check in via GUI</t>
-  </si>
-  <si>
     <t>Allow Customers to check in media via GUI</t>
   </si>
   <si>
-    <t>Create Dialog box to allow Check out via GUI</t>
-  </si>
-  <si>
     <t>Allows Customers to check out media via GUI</t>
   </si>
   <si>
-    <t>Create Dialog box to allow customers to pay balance via GUI</t>
-  </si>
-  <si>
     <t>Allows Customers to pay a balance via GUI</t>
   </si>
   <si>
     <t>Allow the Library Manament system to utilize a menu bar for various functions</t>
   </si>
   <si>
-    <t>Implement a menu bar</t>
-  </si>
-  <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Test if Customers can be created via GUI</t>
+  </si>
+  <si>
+    <t>Test if Librarians can be created via GUI</t>
+  </si>
+  <si>
+    <t>Test if check in can be done via GUI</t>
+  </si>
+  <si>
+    <t>Test if check out can be done via GUI</t>
+  </si>
+  <si>
+    <t>Test if pay balance can be done via GUI</t>
+  </si>
+  <si>
+    <t>Test Menu bar</t>
   </si>
 </sst>
 </file>
@@ -2600,28 +2588,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6857,10 +6845,10 @@
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7842,7 +7830,7 @@
         <v>14</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="D34" s="4">
         <v>4</v>
@@ -7869,7 +7857,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="D35" s="4">
         <v>4</v>
@@ -7896,7 +7884,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D36" s="4">
         <v>4</v>
@@ -7923,7 +7911,7 @@
         <v>17</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
       <c r="D37" s="4">
         <v>4</v>
@@ -8252,8 +8240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9115,7 +9103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="113" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="113" workbookViewId="0">
       <selection activeCell="A48" sqref="A48:H48"/>
     </sheetView>
   </sheetViews>
@@ -10007,13 +9995,13 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD22"/>
+      <selection activeCell="G18" sqref="G18:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -10148,7 +10136,7 @@
         <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
         <v>125</v>
@@ -10157,10 +10145,10 @@
         <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G18" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -10169,10 +10157,10 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
         <v>125</v>
@@ -10181,10 +10169,10 @@
         <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G19" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -10193,10 +10181,10 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C20" t="s">
-        <v>166</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
         <v>125</v>
@@ -10205,10 +10193,10 @@
         <v>141</v>
       </c>
       <c r="F20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G20" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -10217,10 +10205,10 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>125</v>
@@ -10229,10 +10217,10 @@
         <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -10271,17 +10259,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -10313,8 +10302,8 @@
         <v>43</v>
       </c>
       <c r="B5">
-        <f>COUNT(A15:A1000)</f>
-        <v>7</v>
+        <f>COUNT(A15:A1007)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -10322,8 +10311,8 @@
         <v>44</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B12" si="0">B5</f>
-        <v>7</v>
+        <f>B5</f>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -10331,8 +10320,8 @@
         <v>45</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>B6-4</f>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -10340,8 +10329,8 @@
         <v>46</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f>B7</f>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -10349,8 +10338,8 @@
         <v>47</v>
       </c>
       <c r="B9" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" ref="B8:B12" si="0">B8</f>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -10359,7 +10348,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -10368,7 +10357,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -10377,7 +10366,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -10411,10 +10400,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
         <v>125</v>
@@ -10423,7 +10412,7 @@
         <v>141</v>
       </c>
       <c r="F18" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G18" t="s">
         <v>157</v>
@@ -10435,34 +10424,34 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
         <v>141</v>
       </c>
       <c r="F19" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" customHeight="1">
       <c r="A20">
-        <f t="shared" ref="A20:A24" si="1">A19+1</f>
+        <f>A19+1</f>
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
         <v>125</v>
@@ -10471,34 +10460,34 @@
         <v>141</v>
       </c>
       <c r="F20" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G20" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16" customHeight="1">
       <c r="A21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A21:A29" si="1">A20+1</f>
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
         <v>141</v>
       </c>
       <c r="F21" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G21" t="s">
-        <v>202</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -10506,23 +10495,23 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>198</v>
+      <c r="B22" t="s">
+        <v>181</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
         <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G22" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -10530,20 +10519,17 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>201</v>
+      <c r="B23" t="s">
+        <v>181</v>
       </c>
       <c r="C23" t="s">
-        <v>182</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F23" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
@@ -10554,25 +10540,182 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>138</v>
+      <c r="B24" t="s">
+        <v>181</v>
       </c>
       <c r="C24" t="s">
-        <v>136</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
         <v>141</v>
       </c>
       <c r="F24" t="s">
+        <v>189</v>
+      </c>
+      <c r="G24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F25" t="s">
+        <v>196</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>128</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" t="s">
+        <v>197</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
+        <v>191</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" t="s">
+        <v>198</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" t="s">
+        <v>134</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" t="s">
         <v>139</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G31" t="s">
         <v>28</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H31" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>